<commit_message>
Final Version (hopefully :-))
</commit_message>
<xml_diff>
--- a/SqlServerScripter/SqlServerScripter/Final-TableList.xlsx
+++ b/SqlServerScripter/SqlServerScripter/Final-TableList.xlsx
@@ -15,7 +15,7 @@
     <sheet name="RealTableList" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RealTableList!$A$1:$G$198</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RealTableList!$A$1:$G$213</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -560,22 +560,22 @@
     <t>tblTimeHistDetail_COAS_pre</t>
   </si>
   <si>
+    <t>tblDeptNames</t>
+  </si>
+  <si>
+    <t>tblEmplAssignments</t>
+  </si>
+  <si>
+    <t>tblEmplNames_Depts</t>
+  </si>
+  <si>
+    <t>tblEmplSites</t>
+  </si>
+  <si>
+    <t>tblEmplSites_Depts</t>
+  </si>
+  <si>
     <t>BIG</t>
-  </si>
-  <si>
-    <t>tblDeptNames</t>
-  </si>
-  <si>
-    <t>tblEmplAssignments</t>
-  </si>
-  <si>
-    <t>tblEmplNames_Depts</t>
-  </si>
-  <si>
-    <t>tblEmplSites</t>
-  </si>
-  <si>
-    <t>tblEmplSites_Depts</t>
   </si>
 </sst>
 </file>
@@ -959,9 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="A214" sqref="A214:XFD220"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5530,109 +5528,109 @@
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D199" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B199" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D199" s="3" t="s">
+      <c r="E199" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F199" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G199" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A200" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A201" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D201" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E199" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F199" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G199" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A200" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D200" s="3" t="s">
+      <c r="E201" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G201" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A202" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D202" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E200" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F200" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G200" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A201" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D201" s="3" t="s">
+      <c r="E202" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A203" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D203" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="E201" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F201" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G201" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A202" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D202" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E202" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F202" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G202" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A203" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C203" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D203" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>17</v>
@@ -5645,124 +5643,124 @@
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A204" s="3" t="s">
+      <c r="A204" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A205" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F205" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A206" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G206" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A207" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D207" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B204" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E204" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F204" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G204" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A205" s="3" t="s">
+      <c r="E207" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A208" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D208" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B205" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D205" s="3" t="s">
+      <c r="E208" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A209" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E205" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F205" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G205" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A206" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D206" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E206" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F206" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G206" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A207" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D207" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E207" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F207" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G207" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A208" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D208" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E208" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F208" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G208" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A209" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="B209" s="3" t="s">
         <v>108</v>
       </c>
@@ -5770,7 +5768,7 @@
         <v>9</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>17</v>
@@ -5783,8 +5781,8 @@
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A210" s="3" t="s">
-        <v>177</v>
+      <c r="A210" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>108</v>
@@ -5793,45 +5791,45 @@
         <v>9</v>
       </c>
       <c r="D210" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A211" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D211" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E210" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F210" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G210" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A211" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D211" s="3" t="s">
+      <c r="E211" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F211" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G211" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A212" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E211" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F211" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G211" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A212" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="B212" s="3" t="s">
         <v>108</v>
       </c>
@@ -5839,21 +5837,21 @@
         <v>9</v>
       </c>
       <c r="D212" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F212" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A213" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="E212" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F212" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G212" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A213" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>108</v>

</xml_diff>